<commit_message>
Wincyj testuf hotfix x2
</commit_message>
<xml_diff>
--- a/Dat/RawData_popsize75.xlsx
+++ b/Dat/RawData_popsize75.xlsx
@@ -1,37 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Python\projekt_korepetycje\Dat\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19572" windowHeight="6468"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Initial minimum</t>
+  </si>
+  <si>
+    <t>Initial maximum</t>
+  </si>
+  <si>
+    <t>Initial average</t>
+  </si>
+  <si>
+    <t>Final minimum</t>
+  </si>
+  <si>
+    <t>Final maximum</t>
+  </si>
+  <si>
+    <t>Final average</t>
+  </si>
+  <si>
+    <t>Minimum income</t>
+  </si>
+  <si>
+    <t>Maximum income</t>
+  </si>
+  <si>
+    <t>Average income</t>
+  </si>
+  <si>
+    <t>Iteration time</t>
+  </si>
+  <si>
+    <t>Suboptimal teaching time</t>
+  </si>
+  <si>
+    <t>Average teaching time</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +92,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,107 +416,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" customWidth="1"/>
+    <col min="12" max="12" width="21.5546875" customWidth="1"/>
+    <col min="13" max="13" width="27.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Initial minimum</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Initial maximum</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Initial average</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Final minimum</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Final maximum</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Final average</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Minimum income</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Maximum income</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Average income</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Iteration time</t>
-        </is>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.02452482424304264</v>
-      </c>
-      <c r="C2" t="n">
-        <v>22.58982722569027</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="B2">
+        <v>2.4524824243042639E-2</v>
+      </c>
+      <c r="C2">
+        <v>22.589827225690271</v>
+      </c>
+      <c r="D2">
         <v>12.60334543131426</v>
       </c>
-      <c r="E2" t="n">
-        <v>34.27439210585162</v>
-      </c>
-      <c r="F2" t="n">
-        <v>35.9439001377977</v>
-      </c>
-      <c r="G2" t="n">
-        <v>35.20249145989857</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="E2">
+        <v>34.274392105851618</v>
+      </c>
+      <c r="F2">
+        <v>35.943900137797698</v>
+      </c>
+      <c r="G2">
+        <v>35.202491459898567</v>
+      </c>
+      <c r="H2">
         <v>143</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>209</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>160.6</v>
       </c>
-      <c r="K2" t="n">
-        <v>19.01895022392273</v>
+      <c r="K2">
+        <v>19.018950223922729</v>
+      </c>
+      <c r="L2">
+        <f>$I2/$F2</f>
+        <v>5.8146166442361347</v>
+      </c>
+      <c r="M2">
+        <f>$J2/$G2</f>
+        <v>4.5621770886003858</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>